<commit_message>
add mgt fee ppt
</commit_message>
<xml_diff>
--- a/mgt_fee/Quarterly_mgt_fee/2021Q4Mgmt.xlsx
+++ b/mgt_fee/Quarterly_mgt_fee/2021Q4Mgmt.xlsx
@@ -4,14 +4,27 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9180"/>
+    <workbookView windowWidth="23040" windowHeight="9180"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -90,7 +103,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
@@ -1063,8 +1076,8 @@
   <sheetPr/>
   <dimension ref="A1:XFD11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -34085,14 +34098,9 @@
       <c r="G9" t="s">
         <v>14</v>
       </c>
-      <c r="H9">
-        <v>8235661.23</v>
-      </c>
-      <c r="I9">
+      <c r="H9"/>
+      <c r="J9">
         <v>4951061.24</v>
-      </c>
-      <c r="J9">
-        <v>13186722.47</v>
       </c>
     </row>
     <row r="10" spans="1:10">

</xml_diff>